<commit_message>
add teacher level and course assignment pages
</commit_message>
<xml_diff>
--- a/templates/grades.xlsx
+++ b/templates/grades.xlsx
@@ -1,31 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akwasi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akwasi\Documents\React\school-portal\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF06D893-8772-4693-9ECA-802EDD33D6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949E7AF8-A17F-4196-91BE-476FCA2EFCCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30465" yWindow="225" windowWidth="17280" windowHeight="8880" xr2:uid="{FDD74CD2-91E3-4BE0-94AC-08D86CD852CF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FDD74CD2-91E3-4BE0-94AC-08D86CD852CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Grades" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>highestMark</t>
   </si>
@@ -86,12 +96,102 @@
   <si>
     <t>Fail</t>
   </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Upper Credit</t>
+  </si>
+  <si>
+    <t>Lower Credit</t>
+  </si>
+  <si>
+    <t>Outstanding</t>
+  </si>
+  <si>
+    <t>Highest</t>
+  </si>
+  <si>
+    <t>Higher</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>High Average</t>
+  </si>
+  <si>
+    <t>Below Average</t>
+  </si>
+  <si>
+    <t>Low Average</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Lower</t>
+  </si>
+  <si>
+    <t>Weak Pass</t>
+  </si>
+  <si>
+    <t>Lowest</t>
+  </si>
+  <si>
+    <t>Distinction</t>
+  </si>
+  <si>
+    <t>Grades</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>A-</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>B-</t>
+  </si>
+  <si>
+    <t>C+</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C-</t>
+  </si>
+  <si>
+    <t>D+</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +209,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,10 +241,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -474,7 +583,7 @@
   <dimension ref="A1:G2156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11383,8 +11492,790 @@
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E9ADB00F-EC49-40AA-8D60-4E31312E2C6E}">
+          <x14:formula1>
+            <xm:f>Data!$A$104:$A$125</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D30</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99DC85E2-0A32-48C2-AC49-4E58ED54813E}">
+          <x14:formula1>
+            <xm:f>Data!$C$104:$C$134</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C30</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B7D42559-94EC-4FF1-BE06-720ADCEFADA7}">
+          <x14:formula1>
+            <xm:f>Data!$A$1:$A$101</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:B30</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D44C307-0BA4-4FF7-B508-DE744D9CD6BA}">
+  <dimension ref="A1:C134"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>20</v>
+      </c>
+      <c r="C103" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C106">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C107">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C108">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C109">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C110">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C111">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C112">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C113" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C114" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C115" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C116" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C117" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C118" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C119" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C120" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C121" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C122" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C123" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C124" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C125" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="3"/>
+      <c r="C126" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="3"/>
+      <c r="C127" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C128" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C129" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C130" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C131" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C132" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C133" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C134" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="RtSSoCYm0bi/QyU+XjaFbEAz+7KXbgLNq3cqwGcWa+5cQzO52wFShUnYRHjKwvAcmu45LXrYMIhiqM7Z981CnQ==" saltValue="AbUS+B1oQgO9YyJlDaQPqQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>